<commit_message>
added notes to transporation-goods.xlsx and summaries to README.md
</commit_message>
<xml_diff>
--- a/excel/transportion-goods.xlsx
+++ b/excel/transportion-goods.xlsx
@@ -8,23 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejwda\Google Drive\01-ejw-data-github\Public\Algorithms\algo-linear-programming\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF1C66E-4E55-43DD-A092-29631CBFF984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CDC4B50-F2DC-4AFA-97A8-4F408682BC5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15750" xr2:uid="{915ABFA8-4B06-AF4F-A2AE-0D5C19EA983C}"/>
+    <workbookView xWindow="-28920" yWindow="1170" windowWidth="29040" windowHeight="15720" xr2:uid="{915ABFA8-4B06-AF4F-A2AE-0D5C19EA983C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Transport Problem 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Factory-Distribution-Decision" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">'Transport Problem 1'!$B$38:$D$40</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">'Factory-Distribution-Decision'!$B$38:$D$40</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">'Transport Problem 1'!$B$38:$D$40</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">'Transport Problem 1'!$F$19:$F$22</definedName>
-    <definedName name="solver_lhs3" localSheetId="0" hidden="1">'Transport Problem 1'!$C$23:$E$23</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">'Factory-Distribution-Decision'!$B$38:$D$40</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">'Factory-Distribution-Decision'!$F$19:$F$22</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">'Factory-Distribution-Decision'!$C$23:$E$23</definedName>
     <definedName name="solver_lin" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
@@ -34,15 +34,15 @@
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">'Transport Problem 1'!$B$42</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">'Factory-Distribution-Decision'!$B$42</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rhs1" localSheetId="0" hidden="1">'Transport Problem 1'!$C$19:$E$21</definedName>
-    <definedName name="solver_rhs2" localSheetId="0" hidden="1">'Transport Problem 1'!$G$19:$G$22</definedName>
-    <definedName name="solver_rhs3" localSheetId="0" hidden="1">'Transport Problem 1'!$C$22:$E$22</definedName>
+    <definedName name="solver_rhs1" localSheetId="0" hidden="1">'Factory-Distribution-Decision'!$C$19:$E$21</definedName>
+    <definedName name="solver_rhs2" localSheetId="0" hidden="1">'Factory-Distribution-Decision'!$G$19:$G$22</definedName>
+    <definedName name="solver_rhs3" localSheetId="0" hidden="1">'Factory-Distribution-Decision'!$C$22:$E$22</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="35">
   <si>
     <t>Capacity</t>
   </si>
@@ -168,6 +168,15 @@
   </si>
   <si>
     <t>3) Constrain that Distribution Table so it can not exceed Demand Table inputs</t>
+  </si>
+  <si>
+    <t>- seems like a constraint on Production between Capacity and Sent might be needed</t>
+  </si>
+  <si>
+    <t>&lt;-- Initially empty; filled in by summarizing Factory Table</t>
+  </si>
+  <si>
+    <t>&lt;-- Initially empty, these are the decision variables</t>
   </si>
 </sst>
 </file>
@@ -244,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -252,29 +261,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2736E5E5-BECC-5346-A216-A9D749F8BA91}">
-  <dimension ref="A1:P42"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -602,7 +601,7 @@
     <col min="1" max="1" width="17.375" customWidth="1"/>
     <col min="5" max="5" width="11.5" customWidth="1"/>
     <col min="7" max="7" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="69" customWidth="1"/>
+    <col min="8" max="8" width="70" customWidth="1"/>
     <col min="11" max="11" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -620,25 +619,25 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="5" t="s">
         <v>28</v>
       </c>
     </row>
@@ -646,7 +645,7 @@
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="8">
         <v>500</v>
       </c>
       <c r="C5" s="2">
@@ -658,10 +657,10 @@
         <v>140</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" ref="D5:E5" si="0">SUM(E27:E29)</f>
+        <f t="shared" ref="E5" si="0">SUM(E27:E29)</f>
         <v>280</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="8">
         <f>SUM(C27:E29)</f>
         <v>500</v>
       </c>
@@ -673,7 +672,7 @@
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="8">
         <v>500</v>
       </c>
       <c r="C6" s="2">
@@ -688,7 +687,7 @@
         <f t="shared" si="1"/>
         <v>135</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="8">
         <f>SUM(C30:E32)</f>
         <v>335</v>
       </c>
@@ -709,21 +708,24 @@
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
+      <c r="H8" s="11" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="7" t="s">
         <v>14</v>
       </c>
     </row>
@@ -829,35 +831,31 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="7" t="s">
         <v>7</v>
       </c>
       <c r="I18" s="1"/>
@@ -865,174 +863,147 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="8">
         <v>50</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D19" s="8">
         <v>80</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E19" s="8">
         <v>200</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="8">
         <f>SUM(C19:E19)</f>
         <v>330</v>
       </c>
-      <c r="G19" s="11">
+      <c r="G19" s="8">
         <f>SUM(B38:D38)</f>
         <v>330</v>
       </c>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C20" s="8">
         <v>120</v>
       </c>
-      <c r="D20" s="11">
+      <c r="D20" s="8">
         <v>80</v>
       </c>
-      <c r="E20" s="11">
+      <c r="E20" s="8">
         <v>40</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="8">
         <f t="shared" ref="F20:F21" si="2">SUM(C20:E20)</f>
         <v>240</v>
       </c>
-      <c r="G20" s="11">
-        <f t="shared" ref="G20:G22" si="3">SUM(B39:D39)</f>
+      <c r="G20" s="8">
+        <f t="shared" ref="G20:G21" si="3">SUM(B39:D39)</f>
         <v>240</v>
       </c>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C21" s="8">
         <v>30</v>
       </c>
-      <c r="D21" s="11">
+      <c r="D21" s="8">
         <v>60</v>
       </c>
-      <c r="E21" s="11">
+      <c r="E21" s="8">
         <v>175</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="8">
         <f t="shared" si="2"/>
         <v>265</v>
       </c>
-      <c r="G21" s="11">
+      <c r="G21" s="8">
         <f t="shared" si="3"/>
         <v>265</v>
       </c>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B22" s="19" t="s">
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="15">
+      <c r="C22" s="2">
         <f>SUM(C19:C21)</f>
         <v>200</v>
       </c>
-      <c r="D22" s="15">
+      <c r="D22" s="2">
         <f>SUM(D19:D21)</f>
         <v>220</v>
       </c>
-      <c r="E22" s="15">
-        <f t="shared" ref="D22:F22" si="4">SUM(E19:E21)</f>
+      <c r="E22" s="2">
+        <f t="shared" ref="E22:F22" si="4">SUM(E19:E21)</f>
         <v>415</v>
       </c>
-      <c r="F22" s="15">
+      <c r="F22" s="2">
         <f t="shared" si="4"/>
         <v>835</v>
       </c>
-      <c r="G22" s="11">
+      <c r="G22" s="2">
         <v>0</v>
       </c>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B23" s="18"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" t="s">
         <v>27</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+      <c r="H25" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D26" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="E26" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="15">
+      <c r="C27" s="2">
         <v>50</v>
       </c>
       <c r="D27" s="2">
@@ -1042,14 +1013,14 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="15">
+      <c r="C28" s="2">
         <v>0</v>
       </c>
       <c r="D28" s="2">
@@ -1059,14 +1030,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C29" s="15">
+      <c r="C29" s="2">
         <v>30</v>
       </c>
       <c r="D29" s="2">
@@ -1076,14 +1047,14 @@
         <v>175</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="15">
+      <c r="C30" s="2">
         <v>0</v>
       </c>
       <c r="D30" s="2">
@@ -1093,14 +1064,14 @@
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C31" s="15">
+      <c r="C31" s="2">
         <v>120</v>
       </c>
       <c r="D31" s="2">
@@ -1110,14 +1081,14 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C32" s="15">
+      <c r="C32" s="2">
         <v>0</v>
       </c>
       <c r="D32" s="2">
@@ -1127,36 +1098,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B35" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="8" t="s">
+      <c r="H35" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C37" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D37" s="9" t="s">
+      <c r="D37" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>1</v>
       </c>
@@ -1170,7 +1144,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>16</v>
       </c>
@@ -1184,7 +1158,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>3</v>
       </c>
@@ -1198,11 +1172,11 @@
         <v>175</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>6</v>
       </c>
-      <c r="B42" s="16">
+      <c r="B42" s="10">
         <f>SUMPRODUCT(C27:E32, C10:E15)</f>
         <v>54150</v>
       </c>
@@ -1210,7 +1184,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="D5:D6 C5:C6 E5:E6" formulaRange="1"/>
+    <ignoredError sqref="D5:D6 E5:E6" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added Excel production scheduling example and updated documentation and README.md
</commit_message>
<xml_diff>
--- a/excel/transportion-goods.xlsx
+++ b/excel/transportion-goods.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejwda\Google Drive\01-ejw-data-github\Public\Algorithms\algo-linear-programming\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CDC4B50-F2DC-4AFA-97A8-4F408682BC5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{274DE39A-2AE3-452A-9794-AB53C1BF70F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1170" windowWidth="29040" windowHeight="15720" xr2:uid="{915ABFA8-4B06-AF4F-A2AE-0D5C19EA983C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{915ABFA8-4B06-AF4F-A2AE-0D5C19EA983C}"/>
   </bookViews>
   <sheets>
     <sheet name="Factory-Distribution-Decision" sheetId="1" r:id="rId1"/>
@@ -72,15 +72,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="34">
   <si>
     <t>Capacity</t>
   </si>
   <si>
     <t>Australia</t>
-  </si>
-  <si>
-    <t>Sweeden</t>
   </si>
   <si>
     <t>Brazil</t>
@@ -593,7 +590,7 @@
   <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -607,43 +604,43 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>14</v>
-      </c>
       <c r="F4" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="8">
         <v>500</v>
@@ -665,12 +662,12 @@
         <v>500</v>
       </c>
       <c r="H5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="8">
         <v>500</v>
@@ -692,46 +689,46 @@
         <v>335</v>
       </c>
       <c r="H6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="H8" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>1</v>
@@ -748,10 +745,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="2">
         <v>80</v>
@@ -765,10 +762,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12" s="2">
         <v>50</v>
@@ -782,7 +779,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>1</v>
@@ -799,10 +796,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="2">
         <v>50</v>
@@ -816,10 +813,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C15" s="2">
         <v>80</v>
@@ -833,30 +830,30 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D18" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="7" t="s">
-        <v>14</v>
-      </c>
       <c r="F18" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -865,7 +862,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>1</v>
@@ -890,10 +887,10 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C20" s="8">
         <v>120</v>
@@ -915,10 +912,10 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C21" s="8">
         <v>30</v>
@@ -940,7 +937,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C22" s="2">
         <f>SUM(C19:C21)</f>
@@ -967,38 +964,38 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="H25" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D26" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>1</v>
@@ -1015,10 +1012,10 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C28" s="2">
         <v>0</v>
@@ -1032,10 +1029,10 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C29" s="2">
         <v>30</v>
@@ -1049,7 +1046,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>1</v>
@@ -1066,10 +1063,10 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C31" s="2">
         <v>120</v>
@@ -1083,10 +1080,10 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C32" s="2">
         <v>0</v>
@@ -1100,34 +1097,34 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H35" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B36" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C37" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -1146,7 +1143,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B39" s="3">
         <v>120</v>
@@ -1160,7 +1157,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B40" s="3">
         <v>30</v>
@@ -1174,7 +1171,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B42" s="10">
         <f>SUMPRODUCT(C27:E32, C10:E15)</f>

</xml_diff>

<commit_message>
updated README.md, fixed comment spelling errors and color coding, added production-scheduling examples
</commit_message>
<xml_diff>
--- a/excel/transportion-goods.xlsx
+++ b/excel/transportion-goods.xlsx
@@ -8,21 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejwda\Google Drive\01-ejw-data-github\Public\Algorithms\algo-linear-programming\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{274DE39A-2AE3-452A-9794-AB53C1BF70F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C63AF8-5539-4AEE-9591-23A034840E89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{915ABFA8-4B06-AF4F-A2AE-0D5C19EA983C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{915ABFA8-4B06-AF4F-A2AE-0D5C19EA983C}"/>
   </bookViews>
   <sheets>
     <sheet name="Factory-Distribution-Decision" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">'Factory-Distribution-Decision'!$B$38:$D$40</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">'Factory-Distribution-Decision'!$B$37:$D$39</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">'Factory-Distribution-Decision'!$B$38:$D$40</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">'Factory-Distribution-Decision'!$B$37:$D$39</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">'Factory-Distribution-Decision'!$F$19:$F$22</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">'Factory-Distribution-Decision'!$C$23:$E$23</definedName>
     <definedName name="solver_lin" localSheetId="0" hidden="1">1</definedName>
@@ -34,7 +34,7 @@
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">'Factory-Distribution-Decision'!$B$42</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">'Factory-Distribution-Decision'!$B$41</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">3</definedName>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="36">
   <si>
     <t>Capacity</t>
   </si>
@@ -89,9 +89,6 @@
     <t>Factory1</t>
   </si>
   <si>
-    <t>Objective Function</t>
-  </si>
-  <si>
     <t>Sent</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
     <t>Factory2</t>
   </si>
   <si>
-    <t>Products</t>
-  </si>
-  <si>
     <t>Table</t>
   </si>
   <si>
@@ -161,26 +155,38 @@
     <t>2) Vary Distribution Table inputs</t>
   </si>
   <si>
-    <t>4) Constrain the Demand Total to be greater than the number Sent</t>
-  </si>
-  <si>
     <t>3) Constrain that Distribution Table so it can not exceed Demand Table inputs</t>
   </si>
   <si>
     <t>- seems like a constraint on Production between Capacity and Sent might be needed</t>
   </si>
   <si>
-    <t>&lt;-- Initially empty; filled in by summarizing Factory Table</t>
-  </si>
-  <si>
     <t>&lt;-- Initially empty, these are the decision variables</t>
+  </si>
+  <si>
+    <t>Minimum Cost</t>
+  </si>
+  <si>
+    <t>Equation:</t>
+  </si>
+  <si>
+    <t>Cost Table * Distribution Table</t>
+  </si>
+  <si>
+    <t>&lt;-- Objective Function</t>
+  </si>
+  <si>
+    <t>4) Constrain the Demand Total to be greater than or equal to the number Sent</t>
+  </si>
+  <si>
+    <t>&lt;-- Initially empty; filled in by Solver</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -190,6 +196,14 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -218,7 +232,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -250,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -269,8 +283,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2736E5E5-BECC-5346-A216-A9D749F8BA91}">
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -604,20 +619,20 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>0</v>
@@ -626,16 +641,16 @@
         <v>3</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -662,12 +677,12 @@
         <v>500</v>
       </c>
       <c r="H5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="8">
         <v>500</v>
@@ -689,41 +704,41 @@
         <v>335</v>
       </c>
       <c r="H6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H7" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
-      <c r="H8" s="11" t="s">
-        <v>31</v>
+      <c r="H8" s="10" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>21</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -748,7 +763,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C11" s="2">
         <v>80</v>
@@ -779,7 +794,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>1</v>
@@ -796,10 +811,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C14" s="2">
         <v>50</v>
@@ -813,7 +828,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>2</v>
@@ -830,30 +845,30 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>19</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -862,7 +877,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>1</v>
@@ -881,16 +896,16 @@
         <v>330</v>
       </c>
       <c r="G19" s="8">
-        <f>SUM(B38:D38)</f>
+        <f>SUM(B37:D37)</f>
         <v>330</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C20" s="8">
         <v>120</v>
@@ -906,13 +921,13 @@
         <v>240</v>
       </c>
       <c r="G20" s="8">
-        <f t="shared" ref="G20:G21" si="3">SUM(B39:D39)</f>
+        <f t="shared" ref="G20:G21" si="3">SUM(B38:D38)</f>
         <v>240</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>2</v>
@@ -937,7 +952,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C22" s="2">
         <f>SUM(C19:C21)</f>
@@ -964,33 +979,33 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="H25" s="11" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>21</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -1015,7 +1030,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C28" s="2">
         <v>0</v>
@@ -1046,7 +1061,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>1</v>
@@ -1063,10 +1078,10 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C31" s="2">
         <v>120</v>
@@ -1080,7 +1095,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>2</v>
@@ -1097,85 +1112,89 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B35" t="s">
-        <v>25</v>
-      </c>
-      <c r="H35" s="11" t="s">
-        <v>32</v>
+        <v>23</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="6" t="s">
+      <c r="A36" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>13</v>
+      <c r="A37" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="3">
+        <v>50</v>
+      </c>
+      <c r="C37" s="3">
+        <v>80</v>
+      </c>
+      <c r="D37" s="3">
+        <v>200</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B38" s="3">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="C38" s="3">
         <v>80</v>
       </c>
       <c r="D38" s="3">
-        <v>200</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="B39" s="3">
-        <v>120</v>
+        <v>30</v>
       </c>
       <c r="C39" s="3">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="D39" s="3">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B40" s="3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C40" s="3">
-        <v>60</v>
-      </c>
-      <c r="D40" s="3">
-        <v>175</v>
+      <c r="B41" s="12">
+        <f>SUMPRODUCT(C27:E32, C10:E15)</f>
+        <v>54150</v>
+      </c>
+      <c r="H41" s="10" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>5</v>
-      </c>
-      <c r="B42" s="10">
-        <f>SUMPRODUCT(C27:E32, C10:E15)</f>
-        <v>54150</v>
+        <v>31</v>
+      </c>
+      <c r="B42" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>